<commit_message>
checkpoint 27/02. plot n_obs check
</commit_message>
<xml_diff>
--- a/data/scenario_data.xlsx
+++ b/data/scenario_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -58,100 +58,82 @@
     <t>VisibleWest</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>(B, 12.63), (C, 18.19), (D, 31.86), (E, 52.26), (F, 35.86)</t>
-  </si>
-  <si>
-    <t>(A, 12.63), (C, 25.89), (D, 38.41), (E, 54.41), (F, 44.62)</t>
-  </si>
-  <si>
-    <t>(A, 18.19), (B, 25.89), (D, 46.55), (E, 35.71), (F, 18.73)</t>
-  </si>
-  <si>
-    <t>(A, 31.86), (B, 38.41), (C, 46.55), (E, 82.25), (F, 58.99)</t>
-  </si>
-  <si>
-    <t>(A, 52.26), (B, 54.41), (C, 35.71), (D, 82.25), (F, 30.15)</t>
-  </si>
-  <si>
-    <t>(A, 35.86), (B, 44.62), (C, 18.73), (D, 58.99), (E, 30.15)</t>
-  </si>
-  <si>
-    <t>(obs05, 5.03), (obs10, 8.65)</t>
-  </si>
-  <si>
-    <t>(obs05, 8.34), (obs10, 21.27)</t>
-  </si>
-  <si>
-    <t>(obs01, 10.46), (obs03, 41.94), (obs06, 46.97), (obs10, 16.15)</t>
-  </si>
-  <si>
-    <t>(obs02, 25.31), (obs03, 5.3), (obs07, 27.08), (obs08, 33.54), (obs09, 30.94), (obs10, 30.39)</t>
-  </si>
-  <si>
-    <t>(obs01, 25.99), (obs06, 11.58)</t>
-  </si>
-  <si>
-    <t>(obs01, 19.12)</t>
-  </si>
-  <si>
-    <t>(obs10, 8.65)</t>
-  </si>
-  <si>
-    <t>(obs03, 41.94), (obs10, 16.15)</t>
-  </si>
-  <si>
-    <t>(obs03, 5.3), (obs10, 30.39)</t>
-  </si>
-  <si>
-    <t>(obs01, 25.99)</t>
-  </si>
-  <si>
-    <t>(obs05, 5.03)</t>
-  </si>
-  <si>
-    <t>(obs01, 10.46), (obs06, 46.97)</t>
-  </si>
-  <si>
-    <t>(obs02, 25.31), (obs07, 27.08), (obs08, 33.54), (obs09, 30.94)</t>
-  </si>
-  <si>
-    <t>(obs06, 11.58)</t>
-  </si>
-  <si>
-    <t>(A, 12.63)</t>
-  </si>
-  <si>
-    <t>(D, 46.55)</t>
-  </si>
-  <si>
-    <t>(C, 46.55), (E, 82.25)</t>
-  </si>
-  <si>
-    <t>(C, 35.71), (D, 82.25)</t>
-  </si>
-  <si>
-    <t>(B, 12.63)</t>
-  </si>
-  <si>
-    <t>(E, 35.71)</t>
+    <t>car_01</t>
+  </si>
+  <si>
+    <t>car_02</t>
+  </si>
+  <si>
+    <t>car_03</t>
+  </si>
+  <si>
+    <t>car_04</t>
+  </si>
+  <si>
+    <t>car_05</t>
+  </si>
+  <si>
+    <t>(car_02, 110.05), (car_03, 122.93), (car_04, 67.75), (car_05, 75.01), (car_02, 110.05), (car_03, 122.93), (car_04, 67.75), (car_05, 75.01)</t>
+  </si>
+  <si>
+    <t>(car_01, 110.05), (car_03, 13.09), (car_04, 42.49), (car_05, 35.09), (car_01, 110.05), (car_03, 13.09), (car_04, 42.49), (car_05, 35.09)</t>
+  </si>
+  <si>
+    <t>(car_01, 122.93), (car_02, 13.09), (car_04, 55.51), (car_05, 47.92), (car_01, 122.93), (car_02, 13.09), (car_04, 55.51), (car_05, 47.92)</t>
+  </si>
+  <si>
+    <t>(car_01, 67.75), (car_02, 42.49), (car_03, 55.51), (car_05, 8.67), (car_01, 67.75), (car_02, 42.49), (car_03, 55.51), (car_05, 8.67)</t>
+  </si>
+  <si>
+    <t>(car_01, 75.01), (car_02, 35.09), (car_03, 47.92), (car_04, 8.67), (car_01, 75.01), (car_02, 35.09), (car_03, 47.92), (car_04, 8.67)</t>
+  </si>
+  <si>
+    <t>(obs01, 38.8), (obs02, 5.18), (obs03, 5.71), (obs04, 4.83), (obs05, 24.92), (obs06, 45.9), (obs08, 34.96), (obs09, 2.16), (obs10, 5.02), (obs01, 38.8), (obs02, 5.18), (obs03, 5.71), (obs04, 4.83), (obs05, 24.92), (obs06, 45.9), (obs08, 34.96), (obs09, 2.16), (obs10, 5.02)</t>
+  </si>
+  <si>
+    <t>(obs01, 41.95), (obs06, 22.19), (obs07, 14.0), (obs01, 41.95), (obs06, 22.19), (obs07, 14.0)</t>
+  </si>
+  <si>
+    <t>(obs01, 46.07), (obs06, 30.16), (obs07, 21.65), (obs01, 46.07), (obs06, 30.16), (obs07, 21.65)</t>
+  </si>
+  <si>
+    <t>(obs01, 38.8), (obs01, 38.8)</t>
+  </si>
+  <si>
+    <t>(obs05, 24.92), (obs08, 34.96), (obs05, 24.92), (obs08, 34.96)</t>
+  </si>
+  <si>
+    <t>(obs03, 5.71), (obs04, 4.83), (obs10, 5.02), (obs03, 5.71), (obs04, 4.83), (obs10, 5.02)</t>
+  </si>
+  <si>
+    <t>(obs02, 5.18), (obs06, 45.9), (obs09, 2.16), (obs02, 5.18), (obs06, 45.9), (obs09, 2.16)</t>
+  </si>
+  <si>
+    <t>(car_02, 13.09), (car_02, 13.09)</t>
+  </si>
+  <si>
+    <t>(car_05, 8.67), (car_05, 8.67)</t>
+  </si>
+  <si>
+    <t>(car_03, 13.09), (car_03, 13.09)</t>
+  </si>
+  <si>
+    <t>(car_01, 67.75), (car_01, 67.75)</t>
+  </si>
+  <si>
+    <t>(car_01, 75.01), (car_04, 8.67), (car_01, 75.01), (car_04, 8.67)</t>
+  </si>
+  <si>
+    <t>(car_01, 110.05), (car_04, 42.49), (car_05, 35.09), (car_01, 110.05), (car_04, 42.49), (car_05, 35.09)</t>
+  </si>
+  <si>
+    <t>(car_01, 122.93), (car_04, 55.51), (car_05, 47.92), (car_01, 122.93), (car_04, 55.51), (car_05, 47.92)</t>
+  </si>
+  <si>
+    <t>(car_02, 42.49), (car_03, 55.51), (car_02, 42.49), (car_03, 55.51)</t>
+  </si>
+  <si>
+    <t>(car_02, 35.09), (car_03, 47.92), (car_02, 35.09), (car_03, 47.92)</t>
   </si>
 </sst>
 </file>
@@ -509,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -564,28 +546,34 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>11.00776728570781</v>
+        <v>11.00746188820342</v>
       </c>
       <c r="C2">
-        <v>45.43949243662848</v>
+        <v>45.43949340167618</v>
       </c>
       <c r="D2">
-        <v>90</v>
+        <v>308</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>44</v>
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -593,25 +581,22 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <v>11.00778942155574</v>
+        <v>11.00844905524499</v>
       </c>
       <c r="C3">
-        <v>45.43937903284822</v>
+        <v>45.43961881483433</v>
       </c>
       <c r="D3">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -619,31 +604,22 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>11.00790326324258</v>
+        <v>11.00856714629746</v>
       </c>
       <c r="C4">
-        <v>45.43958604394786</v>
+        <v>45.43961088955921</v>
       </c>
       <c r="D4">
-        <v>180</v>
+        <v>134</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" t="s">
         <v>37</v>
-      </c>
-      <c r="K4" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -651,28 +627,31 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>11.00748426283712</v>
+        <v>11.00806546558897</v>
       </c>
       <c r="C5">
-        <v>45.43954676351245</v>
+        <v>45.43959899859149</v>
       </c>
       <c r="D5">
-        <v>0.1</v>
+        <v>307</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
         <v>34</v>
       </c>
-      <c r="I5" t="s">
+      <c r="N5" t="s">
         <v>38</v>
-      </c>
-      <c r="K5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -680,51 +659,28 @@
         <v>18</v>
       </c>
       <c r="B6">
-        <v>11.00822521153387</v>
+        <v>11.00813626526003</v>
       </c>
       <c r="C6">
-        <v>45.43960992760452</v>
+        <v>45.43956504282627</v>
       </c>
       <c r="D6">
-        <v>180</v>
+        <v>278</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" t="s">
         <v>35</v>
       </c>
-      <c r="I6" t="s">
+      <c r="N6" t="s">
         <v>39</v>
-      </c>
-      <c r="K6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
-        <v>11.00798329807873</v>
-      </c>
-      <c r="C7">
-        <v>45.43973705997001</v>
-      </c>
-      <c r="D7">
-        <v>270</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>